<commit_message>
Uploaded 03-九月-2019 14:06:59 {/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADFEF35-B316-EA43-B9C4-6B7A620532AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AD839B-8078-E343-8DD7-A1985709C5F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37520" yWindow="460" windowWidth="37540" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
+    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,6 @@
   </si>
   <si>
     <t>RULEFLOW-GROUP</t>
-  </si>
-  <si>
-    <t>$Insured: Insured</t>
-  </si>
-  <si>
-    <t>$Insured.setStatus($param)</t>
   </si>
   <si>
     <t>免體檢</t>
@@ -164,6 +158,14 @@
   </si>
   <si>
     <t>nohtc-rule4</t>
+  </si>
+  <si>
+    <t>$insured: Insured</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>$insured.setStatus($param);</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -658,7 +660,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -674,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -687,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -697,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -718,7 +720,7 @@
     </row>
     <row r="5" spans="1:8" ht="16">
       <c r="A5" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -753,7 +755,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -765,16 +767,16 @@
     <row r="8" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -782,19 +784,19 @@
     </row>
     <row r="9" spans="1:8" ht="17">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -802,7 +804,7 @@
     </row>
     <row r="10" spans="1:8" ht="16">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -812,17 +814,17 @@
         <v>1500</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>36</v>
@@ -834,17 +836,17 @@
         <v>800</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="16">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>46</v>
@@ -856,15 +858,15 @@
         <v>350</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>56</v>
@@ -876,10 +878,10 @@
         <v>100</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 18:28:37 {/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02AD839B-8078-E343-8DD7-A1985709C5F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E6C91-9EB9-874F-B5EF-EF45A13C5DBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37520" yWindow="460" windowWidth="37520" windowHeight="21140" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
+    <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>"免體檢"</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>nohealthcheck</t>
   </si>
   <si>
@@ -131,10 +127,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>com.redhat.prudential_poc.pojo.Application,com.redhat.prudential_poc.pojo.Insured</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>保額</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -165,6 +157,14 @@
   </si>
   <si>
     <t>$insured.setStatus($param);</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>"PASS"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>com.redhat.prudential_poc.pojo.Insured</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -660,7 +660,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -755,7 +755,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -776,7 +776,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -784,7 +784,7 @@
     </row>
     <row r="9" spans="1:8" ht="17">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
@@ -793,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -804,7 +804,7 @@
     </row>
     <row r="10" spans="1:8" ht="16">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -814,17 +814,17 @@
         <v>1500</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>36</v>
@@ -836,52 +836,52 @@
         <v>800</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="16">
       <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
         <v>46</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>55</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>350</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16">
       <c r="A13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1">
         <v>56</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>65</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>100</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uploaded 05-九月-2019 23:25:08 {/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
+++ b/src/main/resources/com/redhat/prudential_poc/NoHealthCheck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snowfish/2019_Projects/Prudential/phase2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412E6C91-9EB9-874F-B5EF-EF45A13C5DBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF98E3E-EEA0-3340-AB09-96B364283C19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="460" windowWidth="24880" windowHeight="15540" xr2:uid="{BF831FA7-734E-5742-8418-94B2EC150345}"/>
   </bookViews>
@@ -109,9 +109,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
     <t>age &gt;= $param</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -165,6 +162,10 @@
   </si>
   <si>
     <t>com.redhat.prudential_poc.pojo.Insured</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>amount &lt; $param</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -660,7 +661,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -676,7 +677,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -689,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -755,7 +756,7 @@
     <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -767,16 +768,16 @@
     <row r="8" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -784,7 +785,7 @@
     </row>
     <row r="9" spans="1:8" ht="17">
       <c r="A9" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>10</v>
@@ -793,10 +794,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -804,7 +805,7 @@
     </row>
     <row r="10" spans="1:8" ht="16">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1">
@@ -814,17 +815,17 @@
         <v>1500</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="16">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>36</v>
@@ -836,17 +837,17 @@
         <v>800</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="16">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>46</v>
@@ -858,15 +859,15 @@
         <v>350</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>56</v>
@@ -878,10 +879,10 @@
         <v>100</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>